<commit_message>
Module 2 and 3
</commit_message>
<xml_diff>
--- a/Module_1/Class_3/Class_3_Activities/02-Ins_BasicCharting/Unsolved/ice_cream_faves.xlsx
+++ b/Module_1/Class_3/Class_3_Activities/02-Ins_BasicCharting/Unsolved/ice_cream_faves.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcorless/Documents/coding-boot-camp/DataViz-Lesson-Plans/01-Lesson-Plans/01-Excel/3/Activities/02-Ins_BasicCharting/Unsolved/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06d23b41cf651141/Desktop/Activities/Module_1/Class_3/Class_3_Activities/02-Ins_BasicCharting/Unsolved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF88B0C9-A8A2-CD4F-A105-94A35F5E8DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{FF88B0C9-A8A2-CD4F-A105-94A35F5E8DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67DD0A25-BE74-4B8F-8C17-3BCA1A31FD7B}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1700" windowWidth="14620" windowHeight="14080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -194,6 +199,992 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Faves</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Butter Pecan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mint</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Rainbow Sherbert</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Vanilla</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Strawberry</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rocky Road</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cookie Dough</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Coffee</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Neapolitan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F54D-47B0-BCBF-D2A116EC19F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1112185951"/>
+        <c:axId val="625750735"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1112185951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625750735"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="625750735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1112185951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1008602D-1A75-4A84-391C-F667F51B98F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -511,17 +1502,17 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="8" width="20.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -534,7 +1525,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -546,7 +1537,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -558,7 +1549,7 @@
         <v>0.15666666666666668</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -570,7 +1561,7 @@
         <v>0.13166666666666665</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -582,7 +1573,7 @@
         <v>0.11166666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -594,7 +1585,7 @@
         <v>0.10666666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -606,7 +1597,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -618,7 +1609,7 @@
         <v>8.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -630,7 +1621,7 @@
         <v>6.8333333333333329E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -642,7 +1633,7 @@
         <v>5.6666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -654,12 +1645,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>SUM(B2:B11)</f>
         <v>600</v>
@@ -668,8 +1659,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>